<commit_message>
Re-calibrates total generation in 2023 (BCEU); fixes guaranteed dispatch; calibrates syc of biomass and petroleum to ENTSO-E; calibrates historical generation (RAF); fixes capacity factors for biomass, petroleum, dist solar (SYSHECF about page)
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRaSYC/BAU Heat Rates and Start Year Capacities.xlsx
+++ b/InputData/elec/BHRaSYC/BAU Heat Rates and Start Year Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BHRaSYC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BHRaSYC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8687AB-7D38-4378-BA0B-D970EAA880BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961D91A4-3704-4210-BBB6-EA37A4E99331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9330" yWindow="2535" windowWidth="18600" windowHeight="12270" firstSheet="7" activeTab="9" xr2:uid="{58905A94-BA09-4443-B274-BF752AC962AF}"/>
+    <workbookView xWindow="28875" yWindow="4155" windowWidth="19470" windowHeight="11115" tabRatio="795" firstSheet="3" activeTab="9" xr2:uid="{58905A94-BA09-4443-B274-BF752AC962AF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="13" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="366">
   <si>
     <t>BHRaSYC - BAU Heat Rate and Start Year Capacity</t>
   </si>
@@ -1172,6 +1172,9 @@
   <si>
     <t>Eurostat</t>
   </si>
+  <si>
+    <t>calibrated to 2022 data in calibration sheet</t>
+  </si>
 </sst>
 </file>
 
@@ -1302,7 +1305,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1416,6 +1419,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6F6F6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1566,7 +1575,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1734,6 +1743,9 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2173,22 +2185,22 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="44"/>
-    <col min="3" max="3" width="45.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="44"/>
+    <col min="1" max="2" width="10.81640625" style="44"/>
+    <col min="3" max="3" width="45.26953125" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="44"/>
   </cols>
   <sheetData>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="43" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="45"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="45" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="45"/>
       <c r="C14" s="45" t="s">
         <v>4</v>
@@ -2208,7 +2220,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="45"/>
       <c r="C15" s="45" t="s">
         <v>6</v>
@@ -2217,7 +2229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C16" s="45" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C17" s="45" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C18" s="45" t="s">
         <v>12</v>
       </c>
@@ -2241,7 +2253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C19" s="45" t="s">
         <v>14</v>
       </c>
@@ -2249,97 +2261,97 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C20" s="48"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="74" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="47"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="74" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="47"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="47"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="47"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="75" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="47"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="74"/>
       <c r="C27" s="47"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="74" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="74"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="74"/>
       <c r="C30" s="76" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="74"/>
       <c r="C31" s="76" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="74"/>
       <c r="C32" s="76" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="47"/>
       <c r="C33" s="47"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="47"/>
       <c r="C34" s="47"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="47"/>
       <c r="C35" s="47"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="47"/>
       <c r="C36" s="47"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="47"/>
       <c r="C37" s="47"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38" s="47"/>
       <c r="C38" s="47"/>
     </row>
@@ -2363,19 +2375,19 @@
   </sheetPr>
   <dimension ref="A1:HC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DP1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DM1" activePane="topRight" state="frozen"/>
       <selection activeCell="B25" sqref="B25:HC25"/>
-      <selection pane="topRight" activeCell="DP12" sqref="DP12"/>
+      <selection pane="topRight" activeCell="DP11" sqref="DP11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="211" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="211" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>321</v>
       </c>
@@ -3010,7 +3022,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3727,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -4444,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -5161,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -5878,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>323</v>
       </c>
@@ -6595,7 +6607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -7312,7 +7324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>319</v>
       </c>
@@ -8029,7 +8041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -8746,7 +8758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -9104,9 +9116,8 @@
       <c r="DO10">
         <v>0</v>
       </c>
-      <c r="DP10" s="27">
-        <f>SUMIFS('Start year capacity (MW)'!$C$3:$C$22,'Start year capacity (MW)'!$G$3:$G$22,A10)+SUMIFS('Start year capacity (MW)'!$D$3:$D$22,'Start year capacity (MW)'!$G$3:$G$22,$A10)</f>
-        <v>21045</v>
+      <c r="DP10" s="113">
+        <v>30230</v>
       </c>
       <c r="DQ10">
         <v>0</v>
@@ -9463,7 +9474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -10180,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -10538,9 +10549,8 @@
       <c r="DO12">
         <v>0</v>
       </c>
-      <c r="DP12" s="27">
-        <f>SUMIFS('Start year capacity (MW)'!$C$3:$C$22,'Start year capacity (MW)'!$G$3:$G$22,A12)+SUMIFS('Start year capacity (MW)'!$D$3:$D$22,'Start year capacity (MW)'!$G$3:$G$22,$A12)</f>
-        <v>16954</v>
+      <c r="DP12" s="113">
+        <v>32408</v>
       </c>
       <c r="DQ12">
         <v>0</v>
@@ -10897,7 +10907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>320</v>
       </c>
@@ -11614,7 +11624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -12331,7 +12341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -13048,7 +13058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -13685,7 +13695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -14322,7 +14332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -14959,7 +14969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -15596,7 +15606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -16233,7 +16243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -16870,7 +16880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -17507,7 +17517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -18144,7 +18154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A24" s="77" t="s">
         <v>93</v>
       </c>
@@ -18781,7 +18791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A25" s="77" t="s">
         <v>95</v>
       </c>
@@ -19425,18 +19435,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4627C354-DDA9-459B-B28E-42CFC2029A22}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -19453,7 +19463,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -19470,7 +19480,7 @@
         <v>74886</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -19487,7 +19497,7 @@
         <v>104643</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -19505,7 +19515,7 @@
         <v>126958.739</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -19522,7 +19532,7 @@
         <v>173233</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -19539,7 +19549,7 @@
         <v>162354</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -19556,7 +19566,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -19573,7 +19583,7 @@
         <v>21045</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -19590,7 +19600,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -19607,7 +19617,7 @@
         <v>47210</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -19624,7 +19634,7 @@
         <v>15137</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -19637,11 +19647,11 @@
       <c r="D12" s="6">
         <v>21038.666666666668</v>
       </c>
-      <c r="E12" s="5">
-        <v>16954</v>
+      <c r="E12" s="111">
+        <v>25000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -19658,7 +19668,7 @@
         <v>4346</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -19675,7 +19685,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -19692,7 +19702,7 @@
         <v>159729.6721919495</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -19709,7 +19719,7 @@
         <v>7430.1221289052428</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -19726,7 +19736,7 @@
         <v>13199.205679145252</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -19743,7 +19753,7 @@
         <v>180359</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -19760,7 +19770,7 @@
         <v>114216</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -19777,7 +19787,7 @@
         <v>41683</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
         <v>47</v>
       </c>
@@ -19785,11 +19795,11 @@
         <v>31</v>
       </c>
       <c r="C21" s="53">
-        <f>C6*$B$37</f>
+        <f>C6*$B$38</f>
         <v>40229.82</v>
       </c>
       <c r="D21" s="53">
-        <f t="shared" ref="D21:E21" si="0">D6*$B$37</f>
+        <f t="shared" ref="D21:E21" si="0">D6*$B$38</f>
         <v>46450.8</v>
       </c>
       <c r="E21" s="53">
@@ -19797,7 +19807,7 @@
         <v>55200.36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>48</v>
       </c>
@@ -19805,11 +19815,11 @@
         <v>31</v>
       </c>
       <c r="C22" s="53">
-        <f>C6*$B$38</f>
+        <f>C6*$B$39</f>
         <v>78093.180000000008</v>
       </c>
       <c r="D22" s="53">
-        <f t="shared" ref="D22:E22" si="1">D6*$B$38</f>
+        <f t="shared" ref="D22:E22" si="1">D6*$B$39</f>
         <v>90169.2</v>
       </c>
       <c r="E22" s="53">
@@ -19817,85 +19827,90 @@
         <v>107153.64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="54"/>
       <c r="C23" s="55"/>
       <c r="D23" s="55"/>
       <c r="E23" s="55"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="112" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="57"/>
+      <c r="B33" s="57"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>2022</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="51">
+      <c r="B38" s="51">
         <v>0.34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="51">
+      <c r="B39" s="51">
         <v>0.66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1" display="Source : Solar Power europe : Global Market Outlook 2023-2027, figure 21.1" xr:uid="{F125C04B-08F8-4C65-A324-3D5D743B4E3A}"/>
+    <hyperlink ref="A34" r:id="rId1" display="Source : Solar Power europe : Global Market Outlook 2023-2027, figure 21.1" xr:uid="{F125C04B-08F8-4C65-A324-3D5D743B4E3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19906,21 +19921,21 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="28.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
         <v>60</v>
       </c>
@@ -19938,7 +19953,7 @@
       </c>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -19956,7 +19971,7 @@
         <v>53935</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>28</v>
       </c>
@@ -19974,7 +19989,7 @@
         <v>101730</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>29</v>
       </c>
@@ -19993,7 +20008,7 @@
         <v>139985</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
@@ -20011,7 +20026,7 @@
         <v>162872</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
@@ -20030,7 +20045,7 @@
         <v>136377</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
@@ -20048,7 +20063,7 @@
         <v>12760</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
@@ -20065,7 +20080,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -20083,7 +20098,7 @@
         <v>46171</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
@@ -20097,11 +20112,11 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E12" si="1">B11+C11+D11</f>
+        <f t="shared" ref="E11" si="1">B11+C11+D11</f>
         <v>14535</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
@@ -20115,11 +20130,11 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f>B12+C12+D12</f>
         <v>23097</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
@@ -20136,7 +20151,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>40</v>
       </c>
@@ -20154,7 +20169,7 @@
         <v>10987</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>41</v>
       </c>
@@ -20172,7 +20187,7 @@
         <v>120107</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>42</v>
       </c>
@@ -20190,7 +20205,7 @@
         <v>5587</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>43</v>
       </c>
@@ -20208,7 +20223,7 @@
         <v>9925</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>44</v>
       </c>
@@ -20229,7 +20244,7 @@
         <v>135619</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>32</v>
       </c>
@@ -20245,7 +20260,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>67</v>
       </c>
@@ -20260,7 +20275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="60" t="s">
         <v>47</v>
       </c>
@@ -20278,7 +20293,7 @@
         <v>41693</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="62" t="s">
         <v>48</v>
       </c>
@@ -20296,26 +20311,26 @@
         <v>92380</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
     </row>
   </sheetData>
@@ -20334,19 +20349,19 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="100" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" style="100" customWidth="1"/>
     <col min="2" max="3" width="10" style="100" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="100"/>
+    <col min="4" max="16384" width="9.1796875" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="99" t="s">
         <v>325</v>
       </c>
@@ -20354,7 +20369,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="99" t="s">
         <v>327</v>
       </c>
@@ -20362,8 +20377,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="101" t="s">
         <v>329</v>
       </c>
@@ -20371,7 +20385,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="101" t="s">
         <v>331</v>
       </c>
@@ -20379,7 +20393,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="101" t="s">
         <v>333</v>
       </c>
@@ -20387,7 +20401,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="101" t="s">
         <v>335</v>
       </c>
@@ -20395,7 +20409,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="101" t="s">
         <v>337</v>
       </c>
@@ -20403,8 +20417,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="102" t="s">
         <v>339</v>
       </c>
@@ -20415,7 +20428,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="104" t="s">
         <v>342</v>
       </c>
@@ -20426,7 +20439,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="106" t="s">
         <v>344</v>
       </c>
@@ -20437,7 +20450,7 @@
         <v>884325.67500000005</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="106" t="s">
         <v>345</v>
       </c>
@@ -20448,7 +20461,7 @@
         <v>325702.61800000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="106" t="s">
         <v>346</v>
       </c>
@@ -20459,7 +20472,7 @@
         <v>149613.179</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="106" t="s">
         <v>347</v>
       </c>
@@ -20470,7 +20483,7 @@
         <v>103687.709</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="106" t="s">
         <v>348</v>
       </c>
@@ -20481,7 +20494,7 @@
         <v>23271.03</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="106" t="s">
         <v>349</v>
       </c>
@@ -20492,7 +20505,7 @@
         <v>22654.44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="106" t="s">
         <v>350</v>
       </c>
@@ -20503,7 +20516,7 @@
         <v>874.94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="106" t="s">
         <v>351</v>
       </c>
@@ -20514,7 +20527,7 @@
         <v>186055.20199999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="106" t="s">
         <v>352</v>
       </c>
@@ -20525,7 +20538,7 @@
         <v>26835.149000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="106" t="s">
         <v>353</v>
       </c>
@@ -20536,7 +20549,7 @@
         <v>2470.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="106" t="s">
         <v>354</v>
       </c>
@@ -20547,7 +20560,7 @@
         <v>2306.0129999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="106" t="s">
         <v>355</v>
       </c>
@@ -20558,7 +20571,7 @@
         <v>112962.333</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="106" t="s">
         <v>356</v>
       </c>
@@ -20569,7 +20582,7 @@
         <v>23535.956999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="106" t="s">
         <v>357</v>
       </c>
@@ -20580,7 +20593,7 @@
         <v>91547.933999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="106" t="s">
         <v>358</v>
       </c>
@@ -20591,7 +20604,7 @@
         <v>215.988</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="106" t="s">
         <v>359</v>
       </c>
@@ -20602,7 +20615,7 @@
         <v>105111.59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="106" t="s">
         <v>360</v>
       </c>
@@ -20613,12 +20626,12 @@
         <v>1490.8119999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="101" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="101" t="s">
         <v>362</v>
       </c>
@@ -20636,18 +20649,18 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
         <v>70</v>
       </c>
@@ -20670,7 +20683,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -20697,7 +20710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>28</v>
       </c>
@@ -20724,7 +20737,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>29</v>
       </c>
@@ -20751,7 +20764,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
@@ -20778,7 +20791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
@@ -20802,7 +20815,7 @@
         <v>162354</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
@@ -20829,7 +20842,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
@@ -20856,7 +20869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -20883,7 +20896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
@@ -20910,7 +20923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
@@ -20920,7 +20933,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>16954</v>
+        <v>25000</v>
       </c>
       <c r="D12">
         <f>'Capacity GEXIT 2025'!D12</f>
@@ -20931,13 +20944,13 @@
       </c>
       <c r="F12" s="15">
         <f>'Raw Capacities 2019'!E12</f>
-        <v>16954</v>
+        <v>25000</v>
       </c>
       <c r="G12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
@@ -20964,7 +20977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>40</v>
       </c>
@@ -20988,7 +21001,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>41</v>
       </c>
@@ -21015,7 +21028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>42</v>
       </c>
@@ -21042,7 +21055,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>43</v>
       </c>
@@ -21069,7 +21082,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>44</v>
       </c>
@@ -21093,7 +21106,7 @@
         <v>180359</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>32</v>
       </c>
@@ -21117,7 +21130,7 @@
         <v>162354</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>33</v>
       </c>
@@ -21144,7 +21157,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="60" t="s">
         <v>47</v>
       </c>
@@ -21170,7 +21183,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="62" t="s">
         <v>48</v>
       </c>
@@ -21193,24 +21206,24 @@
         <v>107153.64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G25" s="77"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G26" s="77"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
@@ -21228,20 +21241,20 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
@@ -21258,7 +21271,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -21273,7 +21286,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>28</v>
       </c>
@@ -21293,7 +21306,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
         <v>29</v>
       </c>
@@ -21302,7 +21315,7 @@
       <c r="D5" s="82"/>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
         <v>30</v>
       </c>
@@ -21311,7 +21324,7 @@
       <c r="D6" s="82"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
         <v>65</v>
       </c>
@@ -21320,7 +21333,7 @@
       <c r="D7" s="82"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
@@ -21336,7 +21349,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
         <v>35</v>
       </c>
@@ -21345,7 +21358,7 @@
       <c r="D9" s="82"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -21360,7 +21373,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
         <v>37</v>
       </c>
@@ -21369,7 +21382,7 @@
       <c r="D11" s="82"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
@@ -21384,7 +21397,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
@@ -21399,7 +21412,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="s">
         <v>40</v>
       </c>
@@ -21408,7 +21421,7 @@
       <c r="D14" s="82"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>82</v>
       </c>
@@ -21423,7 +21436,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>83</v>
       </c>
@@ -21438,7 +21451,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>84</v>
       </c>
@@ -21453,7 +21466,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>44</v>
       </c>
@@ -21462,7 +21475,7 @@
       <c r="D18" s="82"/>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>85</v>
       </c>
@@ -21477,7 +21490,7 @@
         <v>0.3412</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>86</v>
       </c>
@@ -21492,7 +21505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>87</v>
       </c>
@@ -21507,7 +21520,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>88</v>
       </c>
@@ -21522,7 +21535,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>89</v>
       </c>
@@ -21537,7 +21550,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>90</v>
       </c>
@@ -21552,7 +21565,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>91</v>
       </c>
@@ -21570,7 +21583,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="85" t="s">
         <v>93</v>
       </c>
@@ -21588,7 +21601,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="86" t="s">
         <v>95</v>
       </c>
@@ -21603,42 +21616,42 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="34" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="41" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="78" t="s">
         <v>101</v>
       </c>
@@ -21658,16 +21671,16 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A15" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="41.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>76</v>
       </c>
@@ -21676,7 +21689,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
         <v>26</v>
       </c>
@@ -21693,7 +21706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
@@ -21711,7 +21724,7 @@
         <v>2.2727272727272729</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>28</v>
       </c>
@@ -21732,7 +21745,7 @@
         <v>2.7027027027027026</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>29</v>
       </c>
@@ -21741,7 +21754,7 @@
       <c r="D5" s="82"/>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
@@ -21750,7 +21763,7 @@
       <c r="D6" s="82"/>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
@@ -21759,7 +21772,7 @@
       <c r="D7" s="82"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
@@ -21777,7 +21790,7 @@
         <v>3.1446540880503142</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
@@ -21786,7 +21799,7 @@
       <c r="D9" s="82"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
@@ -21804,7 +21817,7 @@
         <v>2.4390243902439024</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
@@ -21813,7 +21826,7 @@
       <c r="D11" s="82"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
@@ -21831,7 +21844,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
@@ -21849,7 +21862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>40</v>
       </c>
@@ -21858,7 +21871,7 @@
       <c r="D14" s="82"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>41</v>
       </c>
@@ -21876,7 +21889,7 @@
         <v>1.9230769230769229</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>42</v>
       </c>
@@ -21894,7 +21907,7 @@
         <v>2.9411764705882351</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>43</v>
       </c>
@@ -21912,7 +21925,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>44</v>
       </c>
@@ -21930,7 +21943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>85</v>
       </c>
@@ -21948,7 +21961,7 @@
         <v>2.9308323563892147</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>86</v>
       </c>
@@ -21966,7 +21979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>87</v>
       </c>
@@ -21984,7 +21997,7 @@
         <v>2.7027027027027026</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>88</v>
       </c>
@@ -22002,7 +22015,7 @@
         <v>2.3255813953488373</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>89</v>
       </c>
@@ -22020,7 +22033,7 @@
         <v>3.7037037037037033</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>90</v>
       </c>
@@ -22038,7 +22051,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>91</v>
       </c>
@@ -22056,7 +22069,7 @@
         <v>3.0303030303030303</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="85" t="s">
         <v>93</v>
       </c>
@@ -22074,7 +22087,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="86" t="s">
         <v>95</v>
       </c>
@@ -22092,13 +22105,13 @@
         <v>1.9230769230769229</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
     </row>
   </sheetData>
@@ -22114,12 +22127,12 @@
       <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="41.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
         <v>76</v>
       </c>
@@ -22127,7 +22140,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="68" t="s">
         <v>26</v>
       </c>
@@ -22144,7 +22157,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="68" t="s">
         <v>27</v>
       </c>
@@ -22162,7 +22175,7 @@
         <v>7754863.6363636367</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>28</v>
       </c>
@@ -22183,7 +22196,7 @@
         <v>9222000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>29</v>
       </c>
@@ -22192,7 +22205,7 @@
       <c r="D5" s="90"/>
       <c r="E5" s="73"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>30</v>
       </c>
@@ -22201,7 +22214,7 @@
       <c r="D6" s="90"/>
       <c r="E6" s="73"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>65</v>
       </c>
@@ -22210,7 +22223,7 @@
       <c r="D7" s="92"/>
       <c r="E7" s="73"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>34</v>
       </c>
@@ -22228,7 +22241,7 @@
         <v>10729999.999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>35</v>
       </c>
@@ -22237,7 +22250,7 @@
       <c r="D9" s="92"/>
       <c r="E9" s="73"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>36</v>
       </c>
@@ -22255,7 +22268,7 @@
         <v>8322292.682926829</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>37</v>
       </c>
@@ -22264,7 +22277,7 @@
       <c r="D11" s="92"/>
       <c r="E11" s="73"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>38</v>
       </c>
@@ -22282,7 +22295,7 @@
         <v>9748971.4285714291</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>39</v>
       </c>
@@ -22300,7 +22313,7 @@
         <v>17060700</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>40</v>
       </c>
@@ -22309,7 +22322,7 @@
       <c r="D14" s="92"/>
       <c r="E14" s="73"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>41</v>
       </c>
@@ -22327,7 +22340,7 @@
         <v>6561807.6923076911</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
         <v>42</v>
       </c>
@@ -22345,7 +22358,7 @@
         <v>10035705.882352941</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>43</v>
       </c>
@@ -22363,7 +22376,7 @@
         <v>4549519.9999999991</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>32</v>
       </c>
@@ -22372,7 +22385,7 @@
       <c r="D18" s="90"/>
       <c r="E18" s="73"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>33</v>
       </c>
@@ -22381,7 +22394,7 @@
       <c r="D19" s="90"/>
       <c r="E19" s="73"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>85</v>
       </c>
@@ -22399,7 +22412,7 @@
         <v>10000410.316529894</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>86</v>
       </c>
@@ -22417,7 +22430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>87</v>
       </c>
@@ -22435,7 +22448,7 @@
         <v>9222000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>88</v>
       </c>
@@ -22453,7 +22466,7 @@
         <v>7935209.3023255812</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>89</v>
       </c>
@@ -22471,7 +22484,7 @@
         <v>12637555.555555552</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>90</v>
       </c>
@@ -22489,7 +22502,7 @@
         <v>10662937.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
         <v>91</v>
       </c>
@@ -22507,7 +22520,7 @@
         <v>10339818.181818182</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="85" t="s">
         <v>93</v>
       </c>
@@ -22525,7 +22538,7 @@
         <v>8530350</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="86" t="s">
         <v>95</v>
       </c>
@@ -22543,13 +22556,13 @@
         <v>6561807.6923076911</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33">
         <f>9684100/(3412*1000)</f>
         <v>2.838247362250879</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34">
         <f>1/C33</f>
         <v>0.35233010811536436</v>
@@ -22573,13 +22586,13 @@
       <selection pane="topRight" activeCell="DP12" sqref="DP12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="211" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="211" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A1" s="95" t="s">
         <v>106</v>
       </c>
@@ -23214,7 +23227,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -23850,7 +23863,7 @@
         <v>7754863.6363636367</v>
       </c>
     </row>
-    <row r="3" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -24486,7 +24499,7 @@
         <v>4549519.9999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -25122,7 +25135,7 @@
         <v>6561807.6923076911</v>
       </c>
     </row>
-    <row r="5" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -25758,7 +25771,7 @@
         <v>9222000</v>
       </c>
     </row>
-    <row r="6" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="97" t="s">
         <v>29</v>
       </c>
@@ -26393,7 +26406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="97" t="s">
         <v>30</v>
       </c>
@@ -27028,7 +27041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="97" t="s">
         <v>319</v>
       </c>
@@ -27663,7 +27676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="97" t="s">
         <v>33</v>
       </c>
@@ -28298,7 +28311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -28934,7 +28947,7 @@
         <v>10729999.999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="97" t="s">
         <v>35</v>
       </c>
@@ -29569,7 +29582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -30205,7 +30218,7 @@
         <v>10000410.316529894</v>
       </c>
     </row>
-    <row r="13" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>320</v>
       </c>
@@ -30841,7 +30854,7 @@
         <v>10035705.882352941</v>
       </c>
     </row>
-    <row r="14" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -31477,7 +31490,7 @@
         <v>8322292.682926829</v>
       </c>
     </row>
-    <row r="15" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:211" s="97" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="97" t="s">
         <v>37</v>
       </c>
@@ -32112,7 +32125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -32748,7 +32761,7 @@
         <v>9748971.4285714291</v>
       </c>
     </row>
-    <row r="17" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -33384,7 +33397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -34020,7 +34033,7 @@
         <v>17060700</v>
       </c>
     </row>
-    <row r="19" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -34656,7 +34669,7 @@
         <v>9222000</v>
       </c>
     </row>
-    <row r="20" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -35292,7 +35305,7 @@
         <v>7935209.3023255812</v>
       </c>
     </row>
-    <row r="21" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -35928,7 +35941,7 @@
         <v>12637555.555555552</v>
       </c>
     </row>
-    <row r="22" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -36564,7 +36577,7 @@
         <v>10662937.5</v>
       </c>
     </row>
-    <row r="23" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -37200,7 +37213,7 @@
         <v>10339818.181818182</v>
       </c>
     </row>
-    <row r="24" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A24" s="77" t="s">
         <v>93</v>
       </c>
@@ -37836,7 +37849,7 @@
         <v>8530350</v>
       </c>
     </row>
-    <row r="25" spans="1:211" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:211" x14ac:dyDescent="0.35">
       <c r="A25" s="77" t="s">
         <v>95</v>
       </c>
@@ -38490,6 +38503,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -38712,15 +38734,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65D5533F-31BC-4F03-AAAA-A9D02BE279DF}">
   <ds:schemaRefs>
@@ -38733,6 +38746,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE53B774-577E-4215-97DA-2991DC7CFD5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62BCA187-4C93-42D0-A2D6-6C2E53429CBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38749,12 +38770,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE53B774-577E-4215-97DA-2991DC7CFD5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>